<commit_message>
We are almost there!
</commit_message>
<xml_diff>
--- a/input/KWA.xlsx
+++ b/input/KWA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20415"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuppevelt\Nextcloud\Documents\ProjectsRepositories\AarhusExperiment\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBF53AE-4BF8-4506-9416-FAEA0183C9C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C6A457-3E8A-4C28-BDCF-3152EC9FE579}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
   <si>
     <t>AAR_T0_0-2cm</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>Nr</t>
   </si>
 </sst>
 </file>
@@ -346,10 +349,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -674,807 +676,884 @@
   <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="V17" sqref="V17:V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AB1" s="2"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>41</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>7.85E-2</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>321</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>38.9</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>2.81</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>3.52</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>11.9</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>30.4</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
       <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>6.54E-2</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>245</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>13.1</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>1.8</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>1.89</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>1.62</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>24.5</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4">
         <v>0.6</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>6.5799999999999997E-2</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>271</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>32.299999999999997</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>2.62</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>3.59</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>8.23</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>28.4</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5">
         <v>1.8</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>7.2800000000000004E-2</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>274</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>26.2</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>2.33</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>2.42</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>3.85</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>33.700000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6">
         <v>3</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>6.6600000000000006E-2</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>259</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>16.899999999999999</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>2.0699999999999998</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>2.02</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>2.4900000000000002</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>26.6</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7">
         <v>4.2</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>6.4299999999999996E-2</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>239</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>13.4</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>1.87</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>1.77</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>1.98</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>23.9</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" t="s">
         <v>42</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.6</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>9.7500000000000003E-2</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>366</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>40.4</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>3.32</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>3.91</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>13</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" t="s">
         <v>42</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1.8</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>8.7900000000000006E-2</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>315</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>34.4</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>2.8</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>3.46</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>8.77</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>34.700000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" t="s">
         <v>42</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>3</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>8.3799999999999999E-2</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>318</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>20.3</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>2.34</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>2.44</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>3.24</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>32.1</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" t="s">
         <v>42</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>4.2</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>6.5699999999999995E-2</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>254</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>14</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>1.81</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>1.94</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>2.27</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>24.7</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" t="s">
         <v>42</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>5.4</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>7.0199999999999999E-2</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>271</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>15</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>1.95</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>2.0499999999999998</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>2.17</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <v>26.1</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>2</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13">
         <v>0.6</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>7.0800000000000002E-2</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>259</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>30.2</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>2.5</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>3.26</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>8.93</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>3</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E14">
         <v>1.8</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>8.0399999999999999E-2</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>300</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>26.6</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>2.6</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>2.8</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>5.87</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <v>30.1</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15">
         <v>3</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>8.3099999999999993E-2</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>304</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>19.899999999999999</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>2.39</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>2.29</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>3.08</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>30.9</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="2">
+      <c r="E16">
         <v>4.2</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>6.7199999999999996E-2</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>239</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>13.4</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>1.8</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>1.71</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>1.87</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" t="s">
         <v>43</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>0.6</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>7.22E-2</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>3.63</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>300</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>37.5</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>2.8</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>3.29</v>
       </c>
-      <c r="S17">
+      <c r="T17">
         <v>10.3</v>
       </c>
       <c r="V17">
+        <v>27.8</v>
+      </c>
+      <c r="W17">
         <v>0.18</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" t="s">
         <v>43</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>1.8</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>3.75</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>300</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>34.5</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>2.67</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>3.33</v>
       </c>
-      <c r="S18">
+      <c r="T18">
         <v>8.94</v>
       </c>
       <c r="V18">
+        <v>29.1</v>
+      </c>
+      <c r="W18">
         <v>0.18</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" t="s">
         <v>43</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>3</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>7.2700000000000001E-2</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>3.67</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>319</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>24.2</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>2.37</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <v>2.59</v>
       </c>
-      <c r="S19">
+      <c r="T19">
         <v>4.37</v>
       </c>
       <c r="V19">
+        <v>29.9</v>
+      </c>
+      <c r="W19">
         <v>0.18</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" t="s">
         <v>43</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>4.2</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>7.2300000000000003E-2</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>3.58</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>311</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>20.100000000000001</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>2.2200000000000002</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <v>2.38</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <v>2.86</v>
       </c>
       <c r="V20">
+        <v>29</v>
+      </c>
+      <c r="W20">
         <v>0.18</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" t="s">
         <v>43</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>5.4</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>7.1800000000000003E-2</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>3.6</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>316</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>18.5</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>2.2000000000000002</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <v>2.37</v>
       </c>
-      <c r="S21">
+      <c r="T21">
         <v>2.5099999999999998</v>
       </c>
       <c r="V21">
+        <v>28.7</v>
+      </c>
+      <c r="W21">
         <v>0.19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
We're almost there, still some captions and a bit of discussion though.
</commit_message>
<xml_diff>
--- a/input/KWA.xlsx
+++ b/input/KWA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuppevelt\Nextcloud\Documents\ProjectsRepositories\AarhusExperiment\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harmv\Nextcloud\Documents\ProjectsRepositories\AarhusExperiment\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C6A457-3E8A-4C28-BDCF-3152EC9FE579}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FAE862-0DB9-4288-A48F-29B36F459236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="7800" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="78">
   <si>
     <t>AAR_T0_0-2cm</t>
   </si>
@@ -175,13 +175,97 @@
   </si>
   <si>
     <t>Nr</t>
+  </si>
+  <si>
+    <t>O1_0-1,2cm</t>
+  </si>
+  <si>
+    <t>O1_1,2-2,4cm</t>
+  </si>
+  <si>
+    <t>O1_2,4-3,6cm</t>
+  </si>
+  <si>
+    <t>O1_3,6-4,8cm</t>
+  </si>
+  <si>
+    <t>O1_4,8-6,0cm</t>
+  </si>
+  <si>
+    <t>S1_0-1,2cm</t>
+  </si>
+  <si>
+    <t>S1_1,2-2,4cm</t>
+  </si>
+  <si>
+    <t>S1_2,4-3,6cm</t>
+  </si>
+  <si>
+    <t>S1_3,6-4,8cm</t>
+  </si>
+  <si>
+    <t>S1_4,8-6,0cm</t>
+  </si>
+  <si>
+    <t>O3_0-1,2cm_241029</t>
+  </si>
+  <si>
+    <t>O3_1,2-2,4cm</t>
+  </si>
+  <si>
+    <t>O3_2,4-3,6cm</t>
+  </si>
+  <si>
+    <t>O3_3,6-4,8cm</t>
+  </si>
+  <si>
+    <t>O3_4,8-6,0cm</t>
+  </si>
+  <si>
+    <t>S3_0-1,2cm</t>
+  </si>
+  <si>
+    <t>S3_1,2-2,4cm</t>
+  </si>
+  <si>
+    <t>S3_2,4-3,6cm</t>
+  </si>
+  <si>
+    <t>S3_3,6-4,8cm</t>
+  </si>
+  <si>
+    <t>O4_0-1,2cm</t>
+  </si>
+  <si>
+    <t>O4_1,2-2,4cm</t>
+  </si>
+  <si>
+    <t>O4_2,4-3,6cm</t>
+  </si>
+  <si>
+    <t>O4_3,6-4,8cm</t>
+  </si>
+  <si>
+    <t>O4_4,8-6,0cm</t>
+  </si>
+  <si>
+    <t>S4_0-1,2cm</t>
+  </si>
+  <si>
+    <t>S4_1,2-2,4cm</t>
+  </si>
+  <si>
+    <t>S4_2,4-3,6cm</t>
+  </si>
+  <si>
+    <t>S4_3,6-4,8cm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +323,12 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -673,15 +763,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB21"/>
+  <dimension ref="A1:AB59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17:V21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -767,7 +857,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -805,7 +895,7 @@
         <v>30.4</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -843,7 +933,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -881,7 +971,7 @@
         <v>28.4</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -919,7 +1009,7 @@
         <v>33.700000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -957,7 +1047,7 @@
         <v>26.6</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -995,7 +1085,7 @@
         <v>23.9</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1033,7 +1123,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1071,7 +1161,7 @@
         <v>34.700000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1109,7 +1199,7 @@
         <v>32.1</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1147,7 +1237,7 @@
         <v>24.7</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1185,7 +1275,7 @@
         <v>26.1</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1223,7 +1313,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1261,7 +1351,7 @@
         <v>30.1</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1299,7 +1389,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1337,7 +1427,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1381,7 +1471,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1425,7 +1515,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1469,7 +1559,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1513,7 +1603,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1557,7 +1647,1680 @@
         <v>0.19</v>
       </c>
     </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22">
+        <v>0.6</v>
+      </c>
+      <c r="F22">
+        <v>7.5600000000000001E-2</v>
+      </c>
+      <c r="H22">
+        <v>3.8</v>
+      </c>
+      <c r="I22">
+        <v>318.10000000000002</v>
+      </c>
+      <c r="N22">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="P22">
+        <v>2.97</v>
+      </c>
+      <c r="Q22">
+        <v>3.504</v>
+      </c>
+      <c r="T22">
+        <v>10.99</v>
+      </c>
+      <c r="V22">
+        <v>28.9</v>
+      </c>
+      <c r="W22">
+        <v>0.19800000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23">
+        <v>0.6</v>
+      </c>
+      <c r="F23">
+        <v>7.17E-2</v>
+      </c>
+      <c r="H23">
+        <v>3.54</v>
+      </c>
+      <c r="I23">
+        <v>306.8</v>
+      </c>
+      <c r="N23">
+        <v>37.6</v>
+      </c>
+      <c r="P23">
+        <v>2.81</v>
+      </c>
+      <c r="Q23">
+        <v>3.3340000000000001</v>
+      </c>
+      <c r="T23">
+        <v>10.41</v>
+      </c>
+      <c r="V23">
+        <v>26.9</v>
+      </c>
+      <c r="W23">
+        <v>0.183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24">
+        <v>1.8</v>
+      </c>
+      <c r="F24">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="H24">
+        <v>3.7</v>
+      </c>
+      <c r="I24">
+        <v>304.10000000000002</v>
+      </c>
+      <c r="N24">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="P24">
+        <v>2.66</v>
+      </c>
+      <c r="Q24">
+        <v>3.3260000000000001</v>
+      </c>
+      <c r="T24">
+        <v>8.83</v>
+      </c>
+      <c r="V24">
+        <v>28</v>
+      </c>
+      <c r="W24">
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25">
+        <v>1.8</v>
+      </c>
+      <c r="F25">
+        <v>7.5899999999999995E-2</v>
+      </c>
+      <c r="H25">
+        <v>3.9</v>
+      </c>
+      <c r="I25">
+        <v>320.60000000000002</v>
+      </c>
+      <c r="N25">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="P25">
+        <v>2.78</v>
+      </c>
+      <c r="Q25">
+        <v>3.4780000000000002</v>
+      </c>
+      <c r="T25">
+        <v>9.17</v>
+      </c>
+      <c r="V25">
+        <v>29.4</v>
+      </c>
+      <c r="W25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>7.5200000000000003E-2</v>
+      </c>
+      <c r="H26">
+        <v>3.77</v>
+      </c>
+      <c r="I26">
+        <v>330.5</v>
+      </c>
+      <c r="N26">
+        <v>24.8</v>
+      </c>
+      <c r="P26">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="Q26">
+        <v>2.6509999999999998</v>
+      </c>
+      <c r="T26">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="V26">
+        <v>29.8</v>
+      </c>
+      <c r="W26">
+        <v>0.20200000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>7.4899999999999994E-2</v>
+      </c>
+      <c r="H27">
+        <v>3.7</v>
+      </c>
+      <c r="I27">
+        <v>322.60000000000002</v>
+      </c>
+      <c r="N27">
+        <v>24.5</v>
+      </c>
+      <c r="P27">
+        <v>2.39</v>
+      </c>
+      <c r="Q27">
+        <v>2.6360000000000001</v>
+      </c>
+      <c r="T27">
+        <v>4.47</v>
+      </c>
+      <c r="V27">
+        <v>29.5</v>
+      </c>
+      <c r="W27">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28">
+        <v>4.2</v>
+      </c>
+      <c r="F28">
+        <v>7.4899999999999994E-2</v>
+      </c>
+      <c r="H28">
+        <v>3.77</v>
+      </c>
+      <c r="I28">
+        <v>326.60000000000002</v>
+      </c>
+      <c r="N28">
+        <v>24.7</v>
+      </c>
+      <c r="P28">
+        <v>2.42</v>
+      </c>
+      <c r="Q28">
+        <v>2.649</v>
+      </c>
+      <c r="T28">
+        <v>4.54</v>
+      </c>
+      <c r="V28">
+        <v>29.9</v>
+      </c>
+      <c r="W28">
+        <v>0.21299999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29">
+        <v>4.2</v>
+      </c>
+      <c r="F29">
+        <v>7.0800000000000002E-2</v>
+      </c>
+      <c r="H29">
+        <v>3.59</v>
+      </c>
+      <c r="I29">
+        <v>311.5</v>
+      </c>
+      <c r="N29">
+        <v>19.5</v>
+      </c>
+      <c r="P29">
+        <v>2.17</v>
+      </c>
+      <c r="Q29">
+        <v>2.3180000000000001</v>
+      </c>
+      <c r="T29">
+        <v>2.81</v>
+      </c>
+      <c r="V29">
+        <v>27.8</v>
+      </c>
+      <c r="W29">
+        <v>0.21199999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30">
+        <v>5.4</v>
+      </c>
+      <c r="F30">
+        <v>7.0499999999999993E-2</v>
+      </c>
+      <c r="H30">
+        <v>3.5</v>
+      </c>
+      <c r="I30">
+        <v>302</v>
+      </c>
+      <c r="N30">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="P30">
+        <v>2.1</v>
+      </c>
+      <c r="Q30">
+        <v>2.246</v>
+      </c>
+      <c r="T30">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="V30">
+        <v>26.6</v>
+      </c>
+      <c r="W30">
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31">
+        <v>5.4</v>
+      </c>
+      <c r="F31">
+        <v>7.4700000000000003E-2</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+      <c r="I31">
+        <v>328.9</v>
+      </c>
+      <c r="N31">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="P31">
+        <v>2.36</v>
+      </c>
+      <c r="Q31">
+        <v>2.5129999999999999</v>
+      </c>
+      <c r="T31">
+        <v>2.69</v>
+      </c>
+      <c r="V31">
+        <v>30.1</v>
+      </c>
+      <c r="W31">
+        <v>0.214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32">
+        <v>0.6</v>
+      </c>
+      <c r="F32">
+        <v>7.51E-2</v>
+      </c>
+      <c r="H32">
+        <v>3.82</v>
+      </c>
+      <c r="I32">
+        <v>313.60000000000002</v>
+      </c>
+      <c r="N32">
+        <v>38.9</v>
+      </c>
+      <c r="P32">
+        <v>2.97</v>
+      </c>
+      <c r="Q32">
+        <v>3.6469999999999998</v>
+      </c>
+      <c r="T32">
+        <v>10.99</v>
+      </c>
+      <c r="V32">
+        <v>29.1</v>
+      </c>
+      <c r="W32">
+        <v>0.19600000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33">
+        <v>0.6</v>
+      </c>
+      <c r="F33">
+        <v>7.0199999999999999E-2</v>
+      </c>
+      <c r="H33">
+        <v>3.58</v>
+      </c>
+      <c r="I33">
+        <v>293.89999999999998</v>
+      </c>
+      <c r="N33">
+        <v>36.1</v>
+      </c>
+      <c r="P33">
+        <v>2.77</v>
+      </c>
+      <c r="Q33">
+        <v>3.391</v>
+      </c>
+      <c r="T33">
+        <v>10.19</v>
+      </c>
+      <c r="V33">
+        <v>27.1</v>
+      </c>
+      <c r="W33">
+        <v>0.182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34">
+        <v>1.8</v>
+      </c>
+      <c r="F34">
+        <v>7.3200000000000001E-2</v>
+      </c>
+      <c r="H34">
+        <v>3.74</v>
+      </c>
+      <c r="I34">
+        <v>305.10000000000002</v>
+      </c>
+      <c r="N34">
+        <v>35.1</v>
+      </c>
+      <c r="P34">
+        <v>2.69</v>
+      </c>
+      <c r="Q34">
+        <v>3.4430000000000001</v>
+      </c>
+      <c r="T34">
+        <v>8.23</v>
+      </c>
+      <c r="V34">
+        <v>30.9</v>
+      </c>
+      <c r="W34">
+        <v>0.193</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35">
+        <v>1.8</v>
+      </c>
+      <c r="F35">
+        <v>7.3099999999999998E-2</v>
+      </c>
+      <c r="H35">
+        <v>3.8</v>
+      </c>
+      <c r="I35">
+        <v>307.7</v>
+      </c>
+      <c r="N35">
+        <v>35.4</v>
+      </c>
+      <c r="P35">
+        <v>2.71</v>
+      </c>
+      <c r="Q35">
+        <v>3.516</v>
+      </c>
+      <c r="T35">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="V35">
+        <v>31</v>
+      </c>
+      <c r="W35">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>7.4099999999999999E-2</v>
+      </c>
+      <c r="H36">
+        <v>3.83</v>
+      </c>
+      <c r="I36">
+        <v>323.89999999999998</v>
+      </c>
+      <c r="N36">
+        <v>22.1</v>
+      </c>
+      <c r="P36">
+        <v>2.37</v>
+      </c>
+      <c r="Q36">
+        <v>2.6190000000000002</v>
+      </c>
+      <c r="T36">
+        <v>3.27</v>
+      </c>
+      <c r="V36">
+        <v>30.6</v>
+      </c>
+      <c r="W36">
+        <v>0.189</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37">
+        <v>7.5899999999999995E-2</v>
+      </c>
+      <c r="H37">
+        <v>3.94</v>
+      </c>
+      <c r="I37">
+        <v>333.7</v>
+      </c>
+      <c r="N37">
+        <v>22.4</v>
+      </c>
+      <c r="P37">
+        <v>2.42</v>
+      </c>
+      <c r="Q37">
+        <v>2.6659999999999999</v>
+      </c>
+      <c r="T37">
+        <v>3.3</v>
+      </c>
+      <c r="V37">
+        <v>31.1</v>
+      </c>
+      <c r="W37">
+        <v>0.21199999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38">
+        <v>4.2</v>
+      </c>
+      <c r="F38">
+        <v>7.6499999999999999E-2</v>
+      </c>
+      <c r="H38">
+        <v>3.91</v>
+      </c>
+      <c r="I38">
+        <v>329.8</v>
+      </c>
+      <c r="N38">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="P38">
+        <v>2.34</v>
+      </c>
+      <c r="Q38">
+        <v>2.7029999999999998</v>
+      </c>
+      <c r="T38">
+        <v>3.21</v>
+      </c>
+      <c r="V38">
+        <v>30</v>
+      </c>
+      <c r="W38">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39">
+        <v>4.2</v>
+      </c>
+      <c r="F39">
+        <v>7.5499999999999998E-2</v>
+      </c>
+      <c r="H39">
+        <v>3.94</v>
+      </c>
+      <c r="I39">
+        <v>334.2</v>
+      </c>
+      <c r="N39">
+        <v>19.5</v>
+      </c>
+      <c r="P39">
+        <v>2.34</v>
+      </c>
+      <c r="Q39">
+        <v>2.6509999999999998</v>
+      </c>
+      <c r="T39">
+        <v>2.76</v>
+      </c>
+      <c r="V39">
+        <v>30</v>
+      </c>
+      <c r="W39">
+        <v>0.21099999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40">
+        <v>5.4</v>
+      </c>
+      <c r="F40">
+        <v>7.3700000000000002E-2</v>
+      </c>
+      <c r="H40">
+        <v>3.82</v>
+      </c>
+      <c r="I40">
+        <v>328.3</v>
+      </c>
+      <c r="N40">
+        <v>19.2</v>
+      </c>
+      <c r="P40">
+        <v>2.29</v>
+      </c>
+      <c r="Q40">
+        <v>2.5819999999999999</v>
+      </c>
+      <c r="T40">
+        <v>2.54</v>
+      </c>
+      <c r="V40">
+        <v>29.2</v>
+      </c>
+      <c r="W40">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41">
+        <v>5.4</v>
+      </c>
+      <c r="F41">
+        <v>7.8E-2</v>
+      </c>
+      <c r="H41">
+        <v>3.98</v>
+      </c>
+      <c r="I41">
+        <v>344</v>
+      </c>
+      <c r="N41">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="P41">
+        <v>2.41</v>
+      </c>
+      <c r="Q41">
+        <v>2.722</v>
+      </c>
+      <c r="T41">
+        <v>2.66</v>
+      </c>
+      <c r="V41">
+        <v>30.9</v>
+      </c>
+      <c r="W41">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42">
+        <v>0.6</v>
+      </c>
+      <c r="F42">
+        <v>7.3300000000000004E-2</v>
+      </c>
+      <c r="H42">
+        <v>3.79</v>
+      </c>
+      <c r="I42">
+        <v>317</v>
+      </c>
+      <c r="N42">
+        <v>26.7</v>
+      </c>
+      <c r="P42">
+        <v>2.52</v>
+      </c>
+      <c r="Q42">
+        <v>2.7170000000000001</v>
+      </c>
+      <c r="T42">
+        <v>4.72</v>
+      </c>
+      <c r="V42">
+        <v>28.7</v>
+      </c>
+      <c r="W42">
+        <v>0.19500000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43">
+        <v>1.8</v>
+      </c>
+      <c r="F43">
+        <v>7.3200000000000001E-2</v>
+      </c>
+      <c r="H43">
+        <v>3.77</v>
+      </c>
+      <c r="I43">
+        <v>318.7</v>
+      </c>
+      <c r="N43">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="P43">
+        <v>2.4</v>
+      </c>
+      <c r="Q43">
+        <v>2.3319999999999999</v>
+      </c>
+      <c r="T43">
+        <v>2.56</v>
+      </c>
+      <c r="V43">
+        <v>28.9</v>
+      </c>
+      <c r="W43">
+        <v>0.21099999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="F44">
+        <v>7.8700000000000006E-2</v>
+      </c>
+      <c r="H44">
+        <v>4.01</v>
+      </c>
+      <c r="I44">
+        <v>338.4</v>
+      </c>
+      <c r="N44">
+        <v>26.4</v>
+      </c>
+      <c r="P44">
+        <v>2.67</v>
+      </c>
+      <c r="Q44">
+        <v>2.9990000000000001</v>
+      </c>
+      <c r="T44">
+        <v>4.78</v>
+      </c>
+      <c r="V44">
+        <v>30.1</v>
+      </c>
+      <c r="W44">
+        <v>0.20499999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45">
+        <v>4.2</v>
+      </c>
+      <c r="F45">
+        <v>7.4200000000000002E-2</v>
+      </c>
+      <c r="H45">
+        <v>3.84</v>
+      </c>
+      <c r="I45">
+        <v>320.39999999999998</v>
+      </c>
+      <c r="N45">
+        <v>26.2</v>
+      </c>
+      <c r="P45">
+        <v>2.6</v>
+      </c>
+      <c r="Q45">
+        <v>2.875</v>
+      </c>
+      <c r="T45">
+        <v>4.93</v>
+      </c>
+      <c r="V45">
+        <v>29.2</v>
+      </c>
+      <c r="W45">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46">
+        <v>5.4</v>
+      </c>
+      <c r="F46">
+        <v>7.9200000000000007E-2</v>
+      </c>
+      <c r="H46">
+        <v>4.12</v>
+      </c>
+      <c r="I46">
+        <v>340.9</v>
+      </c>
+      <c r="N46">
+        <v>28</v>
+      </c>
+      <c r="P46">
+        <v>2.78</v>
+      </c>
+      <c r="Q46">
+        <v>3.0670000000000002</v>
+      </c>
+      <c r="T46">
+        <v>5.15</v>
+      </c>
+      <c r="V46">
+        <v>30.9</v>
+      </c>
+      <c r="W46">
+        <v>0.22900000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47">
+        <v>0.6</v>
+      </c>
+      <c r="F47">
+        <v>7.9799999999999996E-2</v>
+      </c>
+      <c r="H47">
+        <v>3.98</v>
+      </c>
+      <c r="I47">
+        <v>334.9</v>
+      </c>
+      <c r="N47">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="P47">
+        <v>2.99</v>
+      </c>
+      <c r="Q47">
+        <v>3.6970000000000001</v>
+      </c>
+      <c r="T47">
+        <v>8.35</v>
+      </c>
+      <c r="V47">
+        <v>34.5</v>
+      </c>
+      <c r="W47">
+        <v>0.189</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" t="s">
+        <v>42</v>
+      </c>
+      <c r="E48">
+        <v>1.8</v>
+      </c>
+      <c r="F48">
+        <v>7.7600000000000002E-2</v>
+      </c>
+      <c r="H48">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="I48">
+        <v>337.3</v>
+      </c>
+      <c r="N48">
+        <v>30.5</v>
+      </c>
+      <c r="P48">
+        <v>2.75</v>
+      </c>
+      <c r="Q48">
+        <v>2.8839999999999999</v>
+      </c>
+      <c r="T48">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="V48">
+        <v>35.6</v>
+      </c>
+      <c r="W48">
+        <v>0.216</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="F49">
+        <v>7.4200000000000002E-2</v>
+      </c>
+      <c r="H49">
+        <v>3.89</v>
+      </c>
+      <c r="I49">
+        <v>326.5</v>
+      </c>
+      <c r="N49">
+        <v>22.6</v>
+      </c>
+      <c r="P49">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="Q49">
+        <v>2.524</v>
+      </c>
+      <c r="T49">
+        <v>3.03</v>
+      </c>
+      <c r="V49">
+        <v>30.8</v>
+      </c>
+      <c r="W49">
+        <v>0.20899999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" t="s">
+        <v>42</v>
+      </c>
+      <c r="E50">
+        <v>4.2</v>
+      </c>
+      <c r="F50">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="H50">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="I50">
+        <v>337.3</v>
+      </c>
+      <c r="N50">
+        <v>20.3</v>
+      </c>
+      <c r="P50">
+        <v>2.57</v>
+      </c>
+      <c r="Q50">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="T50">
+        <v>2.74</v>
+      </c>
+      <c r="V50">
+        <v>30.6</v>
+      </c>
+      <c r="W50">
+        <v>0.20799999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51">
+        <v>0.6</v>
+      </c>
+      <c r="F51">
+        <v>7.3200000000000001E-2</v>
+      </c>
+      <c r="H51">
+        <v>3.85</v>
+      </c>
+      <c r="I51">
+        <v>306.39999999999998</v>
+      </c>
+      <c r="N51">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="P51">
+        <v>2.85</v>
+      </c>
+      <c r="Q51">
+        <v>3.6259999999999999</v>
+      </c>
+      <c r="T51">
+        <v>9.43</v>
+      </c>
+      <c r="V51">
+        <v>27.2</v>
+      </c>
+      <c r="W51">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" t="s">
+        <v>43</v>
+      </c>
+      <c r="E52">
+        <v>1.8</v>
+      </c>
+      <c r="F52">
+        <v>7.4399999999999994E-2</v>
+      </c>
+      <c r="H52">
+        <v>3.76</v>
+      </c>
+      <c r="I52">
+        <v>314.10000000000002</v>
+      </c>
+      <c r="N52">
+        <v>29.5</v>
+      </c>
+      <c r="P52">
+        <v>2.66</v>
+      </c>
+      <c r="Q52">
+        <v>2.94</v>
+      </c>
+      <c r="T52">
+        <v>5.98</v>
+      </c>
+      <c r="V52">
+        <v>28.8</v>
+      </c>
+      <c r="W52">
+        <v>0.19800000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53" t="s">
+        <v>39</v>
+      </c>
+      <c r="C53" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" t="s">
+        <v>43</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+      <c r="F53">
+        <v>8.1900000000000001E-2</v>
+      </c>
+      <c r="H53">
+        <v>4.12</v>
+      </c>
+      <c r="I53">
+        <v>350.8</v>
+      </c>
+      <c r="N53">
+        <v>24.7</v>
+      </c>
+      <c r="P53">
+        <v>2.69</v>
+      </c>
+      <c r="Q53">
+        <v>2.6850000000000001</v>
+      </c>
+      <c r="T53">
+        <v>3.52</v>
+      </c>
+      <c r="V53">
+        <v>32.4</v>
+      </c>
+      <c r="W53">
+        <v>0.20799999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" t="s">
+        <v>43</v>
+      </c>
+      <c r="E54">
+        <v>4.2</v>
+      </c>
+      <c r="F54">
+        <v>7.2900000000000006E-2</v>
+      </c>
+      <c r="H54">
+        <v>3.83</v>
+      </c>
+      <c r="I54">
+        <v>322.39999999999998</v>
+      </c>
+      <c r="N54">
+        <v>20.5</v>
+      </c>
+      <c r="P54">
+        <v>2.42</v>
+      </c>
+      <c r="Q54">
+        <v>2.3839999999999999</v>
+      </c>
+      <c r="T54">
+        <v>2.58</v>
+      </c>
+      <c r="V54">
+        <v>29.2</v>
+      </c>
+      <c r="W54">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55" t="s">
+        <v>73</v>
+      </c>
+      <c r="D55" t="s">
+        <v>43</v>
+      </c>
+      <c r="E55">
+        <v>5.4</v>
+      </c>
+      <c r="F55">
+        <v>7.2800000000000004E-2</v>
+      </c>
+      <c r="H55">
+        <v>3.76</v>
+      </c>
+      <c r="I55">
+        <v>319.39999999999998</v>
+      </c>
+      <c r="N55">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="P55">
+        <v>2.38</v>
+      </c>
+      <c r="Q55">
+        <v>2.3370000000000002</v>
+      </c>
+      <c r="T55">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="V55">
+        <v>29.6</v>
+      </c>
+      <c r="W55">
+        <v>0.17699999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>3</v>
+      </c>
+      <c r="B56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" t="s">
+        <v>42</v>
+      </c>
+      <c r="E56">
+        <v>0.6</v>
+      </c>
+      <c r="F56">
+        <v>7.4200000000000002E-2</v>
+      </c>
+      <c r="H56">
+        <v>3.85</v>
+      </c>
+      <c r="I56">
+        <v>317.7</v>
+      </c>
+      <c r="N56">
+        <v>35.1</v>
+      </c>
+      <c r="P56">
+        <v>2.79</v>
+      </c>
+      <c r="Q56">
+        <v>3.3969999999999998</v>
+      </c>
+      <c r="T56">
+        <v>6.64</v>
+      </c>
+      <c r="V56">
+        <v>34</v>
+      </c>
+      <c r="W56">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" t="s">
+        <v>75</v>
+      </c>
+      <c r="D57" t="s">
+        <v>42</v>
+      </c>
+      <c r="E57">
+        <v>1.8</v>
+      </c>
+      <c r="F57">
+        <v>7.2400000000000006E-2</v>
+      </c>
+      <c r="H57">
+        <v>3.77</v>
+      </c>
+      <c r="I57">
+        <v>321.39999999999998</v>
+      </c>
+      <c r="N57">
+        <v>26.2</v>
+      </c>
+      <c r="P57">
+        <v>2.56</v>
+      </c>
+      <c r="Q57">
+        <v>2.5390000000000001</v>
+      </c>
+      <c r="T57">
+        <v>3.05</v>
+      </c>
+      <c r="V57">
+        <v>33.5</v>
+      </c>
+      <c r="W57">
+        <v>0.20200000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" t="s">
+        <v>42</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="F58">
+        <v>7.5899999999999995E-2</v>
+      </c>
+      <c r="H58">
+        <v>3.94</v>
+      </c>
+      <c r="I58">
+        <v>337.5</v>
+      </c>
+      <c r="N58">
+        <v>21.9</v>
+      </c>
+      <c r="P58">
+        <v>2.62</v>
+      </c>
+      <c r="Q58">
+        <v>2.577</v>
+      </c>
+      <c r="T58">
+        <v>2.69</v>
+      </c>
+      <c r="V58">
+        <v>32.1</v>
+      </c>
+      <c r="W58">
+        <v>0.20499999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C59" t="s">
+        <v>77</v>
+      </c>
+      <c r="D59" t="s">
+        <v>42</v>
+      </c>
+      <c r="E59">
+        <v>4.2</v>
+      </c>
+      <c r="F59">
+        <v>7.4700000000000003E-2</v>
+      </c>
+      <c r="H59">
+        <v>3.96</v>
+      </c>
+      <c r="I59">
+        <v>336.3</v>
+      </c>
+      <c r="N59">
+        <v>20.5</v>
+      </c>
+      <c r="P59">
+        <v>2.59</v>
+      </c>
+      <c r="Q59">
+        <v>2.536</v>
+      </c>
+      <c r="T59">
+        <v>2.58</v>
+      </c>
+      <c r="V59">
+        <v>30.9</v>
+      </c>
+      <c r="W59">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Version 1.0 finished writing!!
</commit_message>
<xml_diff>
--- a/input/KWA.xlsx
+++ b/input/KWA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harmv\Nextcloud\Documents\ProjectsRepositories\AarhusExperiment\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FAE862-0DB9-4288-A48F-29B36F459236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CFCE8A-19BA-4166-B6E0-BC16B41BC214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="7800" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-26955" yWindow="10365" windowWidth="23040" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -765,7 +765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>

</xml_diff>